<commit_message>
add 杂项 to calc.xls
Signed-off-by: 王邈 <shankerwangmiao@gmail.com>
</commit_message>
<xml_diff>
--- a/calc.xlsx
+++ b/calc.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/cash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/Cash/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="24660" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24660" windowHeight="14960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -103,13 +103,20 @@
   </si>
   <si>
     <t>支出:吃喝玩乐</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>支出:杂项</t>
+    <rPh sb="0" eb="2">
+      <t>za xiang</t>
+    </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -170,27 +177,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008F00"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF008F00"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -484,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -529,10 +516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -554,11 +541,11 @@
         <v>9</v>
       </c>
       <c r="B2" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A2,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A2,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A2,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A2,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A2,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A2,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A2,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A2,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -567,11 +554,11 @@
         <v>14</v>
       </c>
       <c r="B3" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A3,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A3,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A3,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A3,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C3" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A3,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A3,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A3,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A3,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -580,147 +567,160 @@
         <v>13</v>
       </c>
       <c r="B4" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A4,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A4,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A4,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A4,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A4,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A4,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A4,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A4,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A5,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A5,Sheet1!$F$2:$F$65475,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A5,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A5,Sheet1!$F$2:$F$65475,C$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A5,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A5,Sheet1!$F$2:$F$65475,B$1)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A5,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A5,Sheet1!$F$2:$F$65475,C$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A6,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A6,Sheet1!$F$2:$F$65475,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A6,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A6,Sheet1!$F$2:$F$65475,C$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A6,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A6,Sheet1!$F$2:$F$65475,B$1)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A6,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A6,Sheet1!$F$2:$F$65475,C$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
       <c r="B7" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A7,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A7,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A7,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A7,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C7" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A7,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A7,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A7,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A7,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A8,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A8,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A8,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A8,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C8" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A8,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A8,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A8,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A8,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A9,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A9,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A9,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A9,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C9" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A9,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A9,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A9,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A9,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A10,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A10,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A10,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A10,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C10" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A10,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A10,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A10,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A10,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B11" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A11,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A11,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A11,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A11,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C11" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A11,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A11,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A11,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A11,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A12,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A12,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A12,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A12,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C12" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A12,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A12,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A12,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A12,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A13,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A13,Sheet1!$F$2:$F$65475,B$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A13,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A13,Sheet1!$F$2:$F$65475,B$1)</f>
         <v>0</v>
       </c>
       <c r="C13" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A13,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A13,Sheet1!$F$2:$F$65475,C$1)</f>
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A13,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A13,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A14,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A14,Sheet1!$F$2:$F$65475,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A14,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A14,Sheet1!$F$2:$F$65475,C$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A14,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A14,Sheet1!$F$2:$F$65475,B$1)</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <f>SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A14,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A14,Sheet1!$F$2:$F$65475,C$1)</f>
+      <c r="B15" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A15,Sheet1!$F$2:$F$65475,B$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A15,Sheet1!$F$2:$F$65475,B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <f ca="1">SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$E$2:$E$65475,$A15,Sheet1!$F$2:$F$65475,C$1)-SUMIFS(Sheet1!$G$2:$G$65475,Sheet1!$D$2:$D$65475,$A15,Sheet1!$F$2:$F$65475,C$1)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B2:C14">
+  <conditionalFormatting sqref="B2:C15">
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>